<commit_message>
Common math functions: abs(), sqrt().
</commit_message>
<xml_diff>
--- a/operations.xlsx
+++ b/operations.xlsx
@@ -5,17 +5,20 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="392" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName function="true" hidden="false" name="LCM" vbProcedure="true"/>
+  </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="43">
   <si>
     <t>6km</t>
   </si>
@@ -138,18 +141,22 @@
   </si>
   <si>
     <t>600m²/min</t>
+  </si>
+  <si>
+    <t>sqrt(49km²)</t>
+  </si>
+  <si>
+    <t>7000m²</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="1">
     <numFmt formatCode="GENERAL" numFmtId="164"/>
-    <numFmt formatCode="[$R$-416]\ #,##0.00;[RED]\-[$R$-416]\ #,##0.00" numFmtId="165"/>
-    <numFmt formatCode="GENERAL" numFmtId="166"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="5">
     <font>
       <name val="Arial"/>
       <charset val="1"/>
@@ -171,25 +178,6 @@
       <name val="Arial"/>
       <family val="0"/>
       <sz val="10"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <charset val="1"/>
-      <family val="2"/>
-      <b val="true"/>
-      <i val="true"/>
-      <color rgb="00000000"/>
-      <sz val="16"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <charset val="1"/>
-      <family val="2"/>
-      <b val="true"/>
-      <i val="true"/>
-      <color rgb="00000000"/>
-      <sz val="11"/>
-      <u val="single"/>
     </font>
     <font>
       <name val="Arial"/>
@@ -223,7 +211,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="24">
+  <cellStyleXfs count="20">
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="164">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
@@ -247,26 +235,10 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="44"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="4" numFmtId="164">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="4" numFmtId="164">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="90" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="5" numFmtId="164">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="5" numFmtId="165">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="6" numFmtId="164" xfId="0">
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
     </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
@@ -275,22 +247,15 @@
     <xf applyAlignment="true" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="2" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="166" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
   </cellXfs>
-  <cellStyles count="10">
+  <cellStyles count="6">
     <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
     <cellStyle builtinId="3" customBuiltin="false" name="Comma" xfId="15"/>
     <cellStyle builtinId="6" customBuiltin="false" name="Comma [0]" xfId="16"/>
     <cellStyle builtinId="4" customBuiltin="false" name="Currency" xfId="17"/>
     <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
     <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
-    <cellStyle builtinId="54" customBuiltin="true" name="Heading 1" xfId="20"/>
-    <cellStyle builtinId="54" customBuiltin="true" name="Heading1 1" xfId="21"/>
-    <cellStyle builtinId="54" customBuiltin="true" name="Result 1" xfId="22"/>
-    <cellStyle builtinId="54" customBuiltin="true" name="Result2 1" xfId="23"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -300,27 +265,29 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L76"/>
+  <dimension ref="A1:L84"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A33" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <pane activePane="topLeft" topLeftCell="A33" xSplit="0" ySplit="-1"/>
-      <selection activeCell="F49" activeCellId="0" pane="topLeft" sqref="F49"/>
-      <selection activeCell="A33" activeCellId="0" pane="bottomLeft" sqref="A33"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A64" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <pane activePane="topLeft" topLeftCell="A64" xSplit="0" ySplit="-1"/>
+      <selection activeCell="D80" activeCellId="0" pane="topLeft" sqref="D80"/>
+      <selection activeCell="A64" activeCellId="0" pane="bottomLeft" sqref="A64"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.30588235294118"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="2.0156862745098"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.2196078431373"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="2.51764705882353"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.4823529411765"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="2.51764705882353"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.078431372549"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="2.51764705882353"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="2.51764705882353"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="11.843137254902"/>
-    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="8.67450980392157"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.1333333333333"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.2"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="2.03137254901961"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.3098039215686"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="2.53333333333333"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.5882352941176"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="2.53333333333333"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.1529411764706"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="2.53333333333333"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="8.56470588235294"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="2.53333333333333"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="11.9333333333333"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="8.56470588235294"/>
+    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="8.73725490196078"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="1">
@@ -956,13 +923,13 @@
         <v>201168</v>
       </c>
       <c r="E34" s="2"/>
-      <c r="F34" s="4" t="n">
+      <c r="F34" s="2" t="n">
         <v>1</v>
       </c>
       <c r="H34" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="L34" s="5" t="n">
+      <c r="L34" s="4" t="n">
         <f aca="false">F35/B35*B34+F35/D35*D34</f>
         <v>326168</v>
       </c>
@@ -980,7 +947,7 @@
       </c>
       <c r="E35" s="2"/>
       <c r="F35" s="3" t="n">
-        <f aca="false">LCM_ADD(B35,D35)</f>
+        <f aca="false">LCM(B35,D35)</f>
         <v>125</v>
       </c>
       <c r="G35" s="2"/>
@@ -1091,13 +1058,13 @@
         <v>1</v>
       </c>
       <c r="E42" s="2"/>
-      <c r="F42" s="4" t="n">
+      <c r="F42" s="2" t="n">
         <v>1</v>
       </c>
       <c r="H42" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="L42" s="5" t="n">
+      <c r="L42" s="4" t="n">
         <f aca="false">F43/B43*B42+F43/D43*D42</f>
         <v>101</v>
       </c>
@@ -1115,7 +1082,7 @@
       </c>
       <c r="E43" s="2"/>
       <c r="F43" s="3" t="n">
-        <f aca="false">LCM_ADD(B43,D43)</f>
+        <f aca="false">LCM(B43,D43)</f>
         <v>100</v>
       </c>
       <c r="G43" s="2"/>
@@ -1636,6 +1603,80 @@
       <c r="G76" s="2"/>
       <c r="H76" s="3" t="n">
         <v>-1</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="79">
+      <c r="B79" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="80">
+      <c r="A80" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B80" s="2" t="n">
+        <v>49</v>
+      </c>
+      <c r="C80" s="2"/>
+      <c r="D80" s="3" t="n">
+        <f aca="false">SQRT(B80*B81)</f>
+        <v>7000</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="81">
+      <c r="A81" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B81" s="2" t="n">
+        <v>1000000</v>
+      </c>
+      <c r="C81" s="2"/>
+      <c r="D81" s="2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="82">
+      <c r="A82" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B82" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C82" s="2"/>
+      <c r="D82" s="2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="83">
+      <c r="A83" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B83" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C83" s="2"/>
+      <c r="D83" s="3" t="n">
+        <f aca="false">B83/2</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="84">
+      <c r="A84" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="B84" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C84" s="2"/>
+      <c r="D84" s="3" t="n">
+        <f aca="false">B84/2</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>